<commit_message>
Fixed a problem with export from Scholarship Universe. Added new applicant ranking clean up stored procedure.
</commit_message>
<xml_diff>
--- a/Code/R/RWithSQLServer/Example Data/ImportedData/AwardingGroup10.xlsx
+++ b/Code/R/RWithSQLServer/Example Data/ImportedData/AwardingGroup10.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>ScholarshipName</t>
   </si>
@@ -31,9 +31,6 @@
   </si>
   <si>
     <t>ApplicantRanking</t>
-  </si>
-  <si>
-    <t>15000</t>
   </si>
 </sst>
 </file>
@@ -353,7 +350,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -375,92 +374,92 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
+      <c r="B2">
+        <v>15000</v>
       </c>
       <c r="C2">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D2">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
+      <c r="B3">
+        <v>15000</v>
       </c>
       <c r="C3">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D3">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
+      <c r="B4">
+        <v>15000</v>
       </c>
       <c r="C4">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D4">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5">
+        <v>15000</v>
+      </c>
+      <c r="C5">
+        <v>14</v>
+      </c>
+      <c r="D5">
         <v>4</v>
-      </c>
-      <c r="C5">
-        <v>8</v>
-      </c>
-      <c r="D5">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
-      <c r="B6" t="s">
-        <v>4</v>
+      <c r="B6">
+        <v>15000</v>
       </c>
       <c r="C6">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D6">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
-      <c r="B7" t="s">
-        <v>4</v>
+      <c r="B7">
+        <v>15000</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D7">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
-      <c r="B8" t="s">
-        <v>4</v>
+      <c r="B8">
+        <v>15000</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -473,148 +472,148 @@
       <c r="A9">
         <v>1</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9">
+        <v>15000</v>
+      </c>
+      <c r="C9">
         <v>4</v>
       </c>
-      <c r="C9">
-        <v>16</v>
-      </c>
       <c r="D9">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
-      <c r="B10" t="s">
-        <v>4</v>
+      <c r="B10">
+        <v>15000</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D10">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
-      <c r="B11" t="s">
-        <v>4</v>
+      <c r="B11">
+        <v>15000</v>
       </c>
       <c r="C11">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D11">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
-      <c r="B12" t="s">
-        <v>4</v>
+      <c r="B12">
+        <v>15000</v>
       </c>
       <c r="C12">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D12">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
-      <c r="B13" t="s">
-        <v>4</v>
+      <c r="B13">
+        <v>15000</v>
       </c>
       <c r="C13">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D13">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
-      <c r="B14" t="s">
-        <v>4</v>
+      <c r="B14">
+        <v>15000</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
-      <c r="B15" t="s">
-        <v>4</v>
+      <c r="B15">
+        <v>15000</v>
       </c>
       <c r="C15">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D15">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
-      <c r="B16" t="s">
-        <v>4</v>
+      <c r="B16">
+        <v>15000</v>
       </c>
       <c r="C16">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D16">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
-      <c r="B17" t="s">
-        <v>4</v>
+      <c r="B17">
+        <v>15000</v>
       </c>
       <c r="C17">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D17">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18">
+        <v>15000</v>
+      </c>
+      <c r="C18">
+        <v>14</v>
+      </c>
+      <c r="D18">
         <v>4</v>
-      </c>
-      <c r="C18">
-        <v>3</v>
-      </c>
-      <c r="D18">
-        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2</v>
       </c>
-      <c r="B19" t="s">
-        <v>4</v>
+      <c r="B19">
+        <v>15000</v>
       </c>
       <c r="C19">
         <v>18</v>
@@ -627,56 +626,56 @@
       <c r="A20">
         <v>2</v>
       </c>
-      <c r="B20" t="s">
-        <v>4</v>
+      <c r="B20">
+        <v>15000</v>
       </c>
       <c r="C20">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D20">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2</v>
       </c>
-      <c r="B21" t="s">
-        <v>4</v>
+      <c r="B21">
+        <v>15000</v>
       </c>
       <c r="C21">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D21">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2</v>
       </c>
-      <c r="B22" t="s">
-        <v>4</v>
+      <c r="B22">
+        <v>15000</v>
       </c>
       <c r="C22">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D22">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2</v>
       </c>
-      <c r="B23" t="s">
-        <v>4</v>
+      <c r="B23">
+        <v>15000</v>
       </c>
       <c r="C23">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>